<commit_message>
Add missing comma seperators between BAM files in download link
</commit_message>
<xml_diff>
--- a/siftedData.xlsx
+++ b/siftedData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -178,18 +178,12 @@
     <t>GSM1003544</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733778/suppl/GSM733778%5Fhg19%5FwgEncodeBroadHistoneK562H3k9acStdAlnRep1%2Ebam  ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733778/suppl/GSM733778%5Fhg19%5FwgEncodeBroadHistoneK562H3k9acStdAlnRep2%2Ebam</t>
-  </si>
-  <si>
     <t>GSM1003454</t>
   </si>
   <si>
     <t>GSM1010794</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733785/suppl/GSM733785%5Fhg19%5FwgEncodeBroadHistoneHelas3CtcfStdAlnRep1%2Ebam ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733785/suppl/GSM733785%5Fhg19%5FwgEncodeBroadHistoneHelas3CtcfStdAlnRep2%2Ebam</t>
-  </si>
-  <si>
     <t>GSM733785</t>
   </si>
   <si>
@@ -208,27 +202,15 @@
     <t>GSM935395</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733711/suppl/GSM733711%5Fhg19%5FwgEncodeBroadHistoneHelas3H3k36me3StdAlnRep1%2Ebam ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733711/suppl/GSM733711%5Fhg19%5FwgEncodeBroadHistoneHelas3H3k36me3StdAlnRep2%2Ebam</t>
-  </si>
-  <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733682/suppl/GSM733682%5Fhg19%5FwgEncodeBroadHistoneHelas3H3k4me3StdAlnRep1%2Ebam ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733682/suppl/GSM733682%5Fhg19%5FwgEncodeBroadHistoneHelas3H3k4me3StdAlnRep2%2Ebam</t>
-  </si>
-  <si>
     <t>GSM935624</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733651/suppl/GSM733651%5Fhg19%5FwgEncodeBroadHistoneK562H3k4me2StdAlnRep1%2Ebam ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733651/suppl/GSM733651%5Fhg19%5FwgEncodeBroadHistoneK562H3k4me2StdAlnRep2%2Ebam</t>
-  </si>
-  <si>
     <t>GSM733651</t>
   </si>
   <si>
     <t>GSM733719</t>
   </si>
   <si>
-    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733719/suppl/GSM733719%5Fhg19%5FwgEncodeBroadHistoneK562CtcfStdAlnRep1%2Ebam ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733719/suppl/GSM733719%5Fhg19%5FwgEncodeBroadHistoneK562CtcfStdAlnRep2%2Ebam</t>
-  </si>
-  <si>
     <t>GSM822295 done by Vishwanath Iyer lab in UTA, using ChIP-seq</t>
   </si>
   <si>
@@ -242,9 +224,6 @@
   </si>
   <si>
     <t>GSE96439</t>
-  </si>
-  <si>
-    <t>https://www.encodeproject.org/files/ENCFF437IPW/@@download/ENCFF437IPW.bam https://www.encodeproject.org/files/ENCFF278VMX/@@download/ENCFF278VMX.bam</t>
   </si>
   <si>
     <t>File Type</t>
@@ -331,9 +310,6 @@
     <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM958nnn/GSM958737/suppl/GSM958737%5Fhg19%5FwgEncodeCaltechRnaSeqH1hescR1x75dSplicesRep1V2%2Ebam, ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM958nnn/GSM958737/suppl/GSM958737%5Fhg19%5FwgEncodeCaltechRnaSeqH1hescR1x75dSplicesRep1V2%2Ebam%2Ebai%2Egz, ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM958nnn/GSM958737/suppl/GSM958737%5Fhg19%5FwgEncodeCaltechRnaSeqH1hescR1x75dSplicesRep2V2%2Ebam, ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM958nnn/GSM958737/suppl/GSM958737%5Fhg19%5FwgEncodeCaltechRnaSeqH1hescR1x75dSplicesRep2V2%2Ebam%2Ebai%2Egz</t>
   </si>
   <si>
-    <t>H1 hESC</t>
-  </si>
-  <si>
     <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733734/suppl/GSM733734%5Fhg19%5FwgEncodeBroadHistoneHelas3H3k4me2StdAlnRep1%2Ebam, ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733734/suppl/GSM733734%5Fhg19%5FwgEncodeBroadHistoneHelas3H3k4me2StdAlnRep2%2Ebam</t>
   </si>
   <si>
@@ -788,9 +764,6 @@
     <t>GSM803513 is from Richard Myers Lab, Hudson Alpha Institute of Biotechnology.</t>
   </si>
   <si>
-    <t>HeLa S3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Randomly chosen from the samples of the most popular lab. </t>
   </si>
   <si>
@@ -889,6 +862,33 @@
   </si>
   <si>
     <t>Genome Version</t>
+  </si>
+  <si>
+    <t>H1_hESC</t>
+  </si>
+  <si>
+    <t>HeLa_S3</t>
+  </si>
+  <si>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733785/suppl/GSM733785%5Fhg19%5FwgEncodeBroadHistoneHelas3CtcfStdAlnRep1%2Ebam, ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733785/suppl/GSM733785%5Fhg19%5FwgEncodeBroadHistoneHelas3CtcfStdAlnRep2%2Ebam</t>
+  </si>
+  <si>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733711/suppl/GSM733711%5Fhg19%5FwgEncodeBroadHistoneHelas3H3k36me3StdAlnRep1%2Ebam, ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733711/suppl/GSM733711%5Fhg19%5FwgEncodeBroadHistoneHelas3H3k36me3StdAlnRep2%2Ebam</t>
+  </si>
+  <si>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733682/suppl/GSM733682%5Fhg19%5FwgEncodeBroadHistoneHelas3H3k4me3StdAlnRep1%2Ebam, ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733682/suppl/GSM733682%5Fhg19%5FwgEncodeBroadHistoneHelas3H3k4me3StdAlnRep2%2Ebam</t>
+  </si>
+  <si>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733651/suppl/GSM733651%5Fhg19%5FwgEncodeBroadHistoneK562H3k4me2StdAlnRep1%2Ebam, ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733651/suppl/GSM733651%5Fhg19%5FwgEncodeBroadHistoneK562H3k4me2StdAlnRep2%2Ebam</t>
+  </si>
+  <si>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733719/suppl/GSM733719%5Fhg19%5FwgEncodeBroadHistoneK562CtcfStdAlnRep1%2Ebam, ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733719/suppl/GSM733719%5Fhg19%5FwgEncodeBroadHistoneK562CtcfStdAlnRep2%2Ebam</t>
+  </si>
+  <si>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733778/suppl/GSM733778%5Fhg19%5FwgEncodeBroadHistoneK562H3k9acStdAlnRep1%2Ebam, ftp://ftp.ncbi.nlm.nih.gov/geo/samples/GSM733nnn/GSM733778/suppl/GSM733778%5Fhg19%5FwgEncodeBroadHistoneK562H3k9acStdAlnRep2%2Ebam</t>
+  </si>
+  <si>
+    <t>https://www.encodeproject.org/files/ENCFF437IPW/@@download/ENCFF437IPW.bam, https://www.encodeproject.org/files/ENCFF278VMX/@@download/ENCFF278VMX.bam</t>
   </si>
 </sst>
 </file>
@@ -2678,8 +2678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A43"/>
+    <sheetView tabSelected="1" topLeftCell="I82" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="I94" sqref="I94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2713,10 +2713,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>22</v>
@@ -2725,10 +2725,10 @@
         <v>43</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="13" customFormat="1" ht="70">
@@ -2739,7 +2739,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>14</v>
@@ -2751,19 +2751,19 @@
         <v>8</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="30">
@@ -2786,19 +2786,19 @@
         <v>8</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="13" customFormat="1" ht="56">
@@ -2809,7 +2809,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>14</v>
@@ -2821,19 +2821,19 @@
         <v>8</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="13" customFormat="1" ht="56">
@@ -2844,7 +2844,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>14</v>
@@ -2856,19 +2856,19 @@
         <v>8</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="13" customFormat="1" ht="60">
@@ -2879,7 +2879,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>14</v>
@@ -2891,19 +2891,19 @@
         <v>8</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="13" customFormat="1" ht="56">
@@ -2914,7 +2914,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>14</v>
@@ -2926,19 +2926,19 @@
         <v>8</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="13" customFormat="1" ht="42">
@@ -2949,7 +2949,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>14</v>
@@ -2961,19 +2961,19 @@
         <v>8</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="13" customFormat="1" ht="60">
@@ -2996,19 +2996,19 @@
         <v>8</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="13" customFormat="1" ht="30">
@@ -3019,7 +3019,7 @@
         <v>32</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>14</v>
@@ -3031,19 +3031,19 @@
         <v>8</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="13" customFormat="1" ht="30">
@@ -3054,7 +3054,7 @@
         <v>35</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>14</v>
@@ -3066,19 +3066,19 @@
         <v>8</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="13" customFormat="1" ht="30">
@@ -3089,7 +3089,7 @@
         <v>26</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>14</v>
@@ -3101,19 +3101,19 @@
         <v>8</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="7" customFormat="1" ht="15">
@@ -3121,7 +3121,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -3131,7 +3131,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K13" s="1"/>
     </row>
@@ -3143,7 +3143,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>39</v>
@@ -3155,19 +3155,19 @@
         <v>8</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="13" customFormat="1" ht="30">
@@ -3178,7 +3178,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>14</v>
@@ -3190,30 +3190,30 @@
         <v>8</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="A16" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>14</v>
@@ -3225,30 +3225,30 @@
         <v>8</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="13" customFormat="1" ht="30">
       <c r="A17" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>14</v>
@@ -3260,30 +3260,30 @@
         <v>8</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="A18" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>36</v>
@@ -3295,30 +3295,30 @@
         <v>8</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="13" customFormat="1" ht="56">
       <c r="A19" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>21</v>
@@ -3330,30 +3330,30 @@
         <v>8</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="A20" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>38</v>
@@ -3365,30 +3365,30 @@
         <v>8</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="A21" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>37</v>
@@ -3400,30 +3400,30 @@
         <v>8</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="13" customFormat="1" ht="56">
       <c r="A22" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>37</v>
@@ -3435,30 +3435,30 @@
         <v>8</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="A23" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D23" s="16" t="s">
         <v>37</v>
@@ -3470,30 +3470,30 @@
         <v>8</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="13" customFormat="1" ht="42">
       <c r="A24" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>37</v>
@@ -3505,30 +3505,30 @@
         <v>8</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="13" customFormat="1" ht="30">
       <c r="A25" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D25" s="16" t="s">
         <v>14</v>
@@ -3540,30 +3540,30 @@
         <v>8</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="13" customFormat="1" ht="30">
       <c r="A26" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>14</v>
@@ -3575,27 +3575,27 @@
         <v>8</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="7" customFormat="1" ht="15">
-      <c r="A27" s="2" t="s">
-        <v>88</v>
+      <c r="A27" s="16" t="s">
+        <v>265</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -3613,16 +3613,16 @@
     </row>
     <row r="28" spans="1:11" s="13" customFormat="1" ht="112">
       <c r="A28" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>7</v>
@@ -3631,30 +3631,30 @@
         <v>8</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="13" customFormat="1" ht="30">
       <c r="A29" s="16" t="s">
-        <v>88</v>
+        <v>265</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>14</v>
@@ -3666,30 +3666,30 @@
         <v>8</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="A30" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D30" s="16" t="s">
         <v>14</v>
@@ -3701,30 +3701,30 @@
         <v>8</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>49</v>
+        <v>267</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="13" customFormat="1" ht="30">
       <c r="A31" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>14</v>
@@ -3736,30 +3736,30 @@
         <v>8</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="A32" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>14</v>
@@ -3771,30 +3771,30 @@
         <v>8</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="A33" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>14</v>
@@ -3806,30 +3806,30 @@
         <v>8</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>56</v>
+        <v>268</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K33" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="A34" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D34" s="16" t="s">
         <v>14</v>
@@ -3841,30 +3841,30 @@
         <v>8</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>57</v>
+        <v>269</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K34" s="14" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="13" customFormat="1" ht="45">
       <c r="A35" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D35" s="16" t="s">
         <v>14</v>
@@ -3876,30 +3876,30 @@
         <v>8</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="13" customFormat="1" ht="56">
       <c r="A36" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>14</v>
@@ -3911,30 +3911,30 @@
         <v>8</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="13" customFormat="1" ht="56">
       <c r="A37" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>14</v>
@@ -3946,30 +3946,30 @@
         <v>8</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I37" s="18" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="13" customFormat="1" ht="28">
       <c r="A38" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>14</v>
@@ -3981,33 +3981,33 @@
         <v>8</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I38" s="18" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="13" customFormat="1" ht="112">
       <c r="A39" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E39" s="20" t="s">
         <v>7</v>
@@ -4016,30 +4016,30 @@
         <v>8</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K39" s="14" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="13" customFormat="1" ht="28">
       <c r="A40" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>14</v>
@@ -4051,33 +4051,33 @@
         <v>8</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="7" customFormat="1" ht="98">
       <c r="A41" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>7</v>
@@ -4087,23 +4087,23 @@
       </c>
       <c r="G41" s="9"/>
       <c r="H41" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="J41" s="10"/>
       <c r="K41" s="1"/>
     </row>
     <row r="42" spans="1:11" s="13" customFormat="1" ht="28">
       <c r="A42" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>14</v>
@@ -4115,30 +4115,30 @@
         <v>8</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K42" s="13" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="13" customFormat="1" ht="60">
       <c r="A43" s="16" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D43" s="16" t="s">
         <v>6</v>
@@ -4150,19 +4150,19 @@
         <v>8</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J43" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K43" s="14" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4173,7 +4173,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="D44" s="16" t="s">
         <v>6</v>
@@ -4185,19 +4185,19 @@
         <v>8</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I44" s="16" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J44" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4208,7 +4208,7 @@
         <v>10</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="D45" s="16" t="s">
         <v>6</v>
@@ -4220,19 +4220,19 @@
         <v>8</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I45" s="16" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="J45" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="13" customFormat="1" ht="28">
@@ -4243,7 +4243,7 @@
         <v>11</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D46" s="16" t="s">
         <v>6</v>
@@ -4255,19 +4255,19 @@
         <v>8</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I46" s="18" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="J46" s="19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K46" s="13" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4278,7 +4278,7 @@
         <v>12</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D47" s="16" t="s">
         <v>6</v>
@@ -4290,19 +4290,19 @@
         <v>8</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="J47" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K47" s="13" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4313,7 +4313,7 @@
         <v>5</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="D48" s="16" t="s">
         <v>6</v>
@@ -4325,19 +4325,19 @@
         <v>8</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="J48" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K48" s="13" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="13" customFormat="1" ht="45">
@@ -4348,7 +4348,7 @@
         <v>17</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="D49" s="16" t="s">
         <v>6</v>
@@ -4360,19 +4360,19 @@
         <v>8</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="I49" s="16" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="J49" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K49" s="13" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4383,7 +4383,7 @@
         <v>24</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D50" s="16" t="s">
         <v>14</v>
@@ -4395,19 +4395,19 @@
         <v>8</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I50" s="16" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="J50" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4430,19 +4430,19 @@
         <v>8</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I51" s="16" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="J51" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4453,7 +4453,7 @@
         <v>15</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>39</v>
@@ -4465,19 +4465,19 @@
         <v>8</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I52" s="16" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J52" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K52" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4488,7 +4488,7 @@
         <v>33</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>14</v>
@@ -4500,19 +4500,19 @@
         <v>8</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I53" s="16" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="J53" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K53" s="13" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="7" customFormat="1" ht="15">
@@ -4520,7 +4520,7 @@
         <v>4</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="3"/>
@@ -4544,7 +4544,7 @@
         <v>23</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>14</v>
@@ -4556,19 +4556,19 @@
         <v>8</v>
       </c>
       <c r="G55" s="20" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I55" s="18" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K55" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:11" s="7" customFormat="1" ht="56">
@@ -4579,10 +4579,10 @@
         <v>29</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E56" s="9" t="s">
         <v>7</v>
@@ -4591,16 +4591,16 @@
         <v>8</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="K56" s="1"/>
     </row>
@@ -4633,10 +4633,10 @@
         <v>11</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E58" s="12" t="s">
         <v>7</v>
@@ -4645,19 +4645,19 @@
         <v>40</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H58" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I58" s="16" t="s">
-        <v>59</v>
+        <v>270</v>
       </c>
       <c r="J58" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K58" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="13" customFormat="1" ht="60">
@@ -4668,10 +4668,10 @@
         <v>12</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E59" s="12" t="s">
         <v>7</v>
@@ -4680,19 +4680,19 @@
         <v>8</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I59" s="16" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="J59" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K59" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="13" customFormat="1" ht="60">
@@ -4703,10 +4703,10 @@
         <v>23</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E60" s="12" t="s">
         <v>7</v>
@@ -4715,19 +4715,19 @@
         <v>8</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="I60" s="16" t="s">
-        <v>62</v>
+        <v>271</v>
       </c>
       <c r="J60" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K60" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="13" customFormat="1" ht="28">
@@ -4738,7 +4738,7 @@
         <v>29</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D61" s="16" t="s">
         <v>14</v>
@@ -4750,19 +4750,19 @@
         <v>8</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H61" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I61" s="18" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="J61" s="19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K61" s="13" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4773,7 +4773,7 @@
         <v>24</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D62" s="16" t="s">
         <v>14</v>
@@ -4785,19 +4785,19 @@
         <v>8</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I62" s="16" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="J62" s="19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K62" s="13" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4808,7 +4808,7 @@
         <v>26</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D63" s="16" t="s">
         <v>14</v>
@@ -4820,19 +4820,19 @@
         <v>8</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H63" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I63" s="16" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="J63" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K63" s="13" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4843,7 +4843,7 @@
         <v>31</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D64" s="16" t="s">
         <v>14</v>
@@ -4855,19 +4855,19 @@
         <v>8</v>
       </c>
       <c r="G64" s="13" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I64" s="16" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="J64" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K64" s="13" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="13" customFormat="1" ht="60">
@@ -4878,10 +4878,10 @@
         <v>5</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>7</v>
@@ -4890,19 +4890,19 @@
         <v>8</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H65" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I65" s="16" t="s">
-        <v>46</v>
+        <v>272</v>
       </c>
       <c r="J65" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K65" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:11" s="13" customFormat="1" ht="60">
@@ -4913,7 +4913,7 @@
         <v>32</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="D66" s="16" t="s">
         <v>39</v>
@@ -4925,19 +4925,19 @@
         <v>8</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H66" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I66" s="16" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="J66" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K66" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="13" customFormat="1" ht="30">
@@ -4948,7 +4948,7 @@
         <v>25</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D67" s="16" t="s">
         <v>14</v>
@@ -4960,19 +4960,19 @@
         <v>8</v>
       </c>
       <c r="G67" s="13" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I67" s="16" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="J67" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K67" s="13" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="13" customFormat="1" ht="60">
@@ -4983,10 +4983,10 @@
         <v>9</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E68" s="12" t="s">
         <v>7</v>
@@ -4995,19 +4995,19 @@
         <v>8</v>
       </c>
       <c r="G68" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I68" s="16" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="J68" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K68" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="13" customFormat="1" ht="56">
@@ -5015,13 +5015,13 @@
         <v>19</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E69" s="20" t="s">
         <v>7</v>
@@ -5030,19 +5030,19 @@
         <v>8</v>
       </c>
       <c r="G69" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H69" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I69" s="14" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="J69" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K69" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="13" customFormat="1" ht="112">
@@ -5053,10 +5053,10 @@
         <v>15</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E70" s="20" t="s">
         <v>7</v>
@@ -5065,19 +5065,19 @@
         <v>8</v>
       </c>
       <c r="G70" s="20" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="H70" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I70" s="14" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K70" s="14" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="13" customFormat="1" ht="60">
@@ -5088,10 +5088,10 @@
         <v>16</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>7</v>
@@ -5100,19 +5100,19 @@
         <v>8</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H71" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I71" s="16" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="J71" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K71" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="13" customFormat="1" ht="42">
@@ -5123,7 +5123,7 @@
         <v>10</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D72" s="16" t="s">
         <v>14</v>
@@ -5135,19 +5135,19 @@
         <v>8</v>
       </c>
       <c r="G72" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H72" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I72" s="16" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="J72" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K72" s="14" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="73" spans="1:11" s="13" customFormat="1" ht="30">
@@ -5158,7 +5158,7 @@
         <v>11</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D73" s="16" t="s">
         <v>14</v>
@@ -5170,19 +5170,19 @@
         <v>8</v>
       </c>
       <c r="G73" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H73" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I73" s="16" t="s">
-        <v>68</v>
+        <v>273</v>
       </c>
       <c r="J73" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K73" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:11" s="13" customFormat="1" ht="28">
@@ -5193,7 +5193,7 @@
         <v>12</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D74" s="16" t="s">
         <v>14</v>
@@ -5205,19 +5205,19 @@
         <v>8</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H74" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I74" s="18" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="J74" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K74" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="13" customFormat="1" ht="28">
@@ -5228,7 +5228,7 @@
         <v>5</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D75" s="16" t="s">
         <v>14</v>
@@ -5240,19 +5240,19 @@
         <v>8</v>
       </c>
       <c r="G75" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H75" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I75" s="18" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="J75" s="19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K75" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="13" customFormat="1" ht="30">
@@ -5263,7 +5263,7 @@
         <v>32</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="D76" s="16" t="s">
         <v>14</v>
@@ -5275,19 +5275,19 @@
         <v>8</v>
       </c>
       <c r="G76" s="12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H76" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I76" s="16" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="J76" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K76" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="13" customFormat="1" ht="30">
@@ -5298,7 +5298,7 @@
         <v>24</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D77" s="16" t="s">
         <v>14</v>
@@ -5310,19 +5310,19 @@
         <v>8</v>
       </c>
       <c r="G77" s="12" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H77" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I77" s="16" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="J77" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K77" s="13" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="13" customFormat="1" ht="60">
@@ -5333,7 +5333,7 @@
         <v>26</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D78" s="16" t="s">
         <v>14</v>
@@ -5345,19 +5345,19 @@
         <v>8</v>
       </c>
       <c r="G78" s="13" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H78" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I78" s="16" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="J78" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K78" s="13" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="7" customFormat="1">
@@ -5382,10 +5382,10 @@
         <v>15</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="D80" s="20" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E80" s="20" t="s">
         <v>7</v>
@@ -5394,19 +5394,19 @@
         <v>8</v>
       </c>
       <c r="G80" s="23" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I80" s="18" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K80" s="13" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="7" customFormat="1" ht="15">
@@ -5414,7 +5414,7 @@
         <v>18</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>7</v>
@@ -5433,7 +5433,7 @@
         <v>9</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D82" s="13" t="s">
         <v>14</v>
@@ -5445,19 +5445,19 @@
         <v>8</v>
       </c>
       <c r="G82" s="23" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="H82" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I82" s="14" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="J82" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K82" s="13" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="13" customFormat="1" ht="28">
@@ -5468,7 +5468,7 @@
         <v>16</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="D83" s="13" t="s">
         <v>14</v>
@@ -5480,19 +5480,19 @@
         <v>8</v>
       </c>
       <c r="G83" s="20" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H83" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I83" s="14" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="J83" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K83" s="14" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="13" customFormat="1" ht="28">
@@ -5503,7 +5503,7 @@
         <v>23</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="D84" s="13" t="s">
         <v>14</v>
@@ -5515,19 +5515,19 @@
         <v>8</v>
       </c>
       <c r="G84" s="20" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H84" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I84" s="14" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="J84" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K84" s="14" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="85" spans="1:11" s="13" customFormat="1" ht="28">
@@ -5538,7 +5538,7 @@
         <v>29</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="D85" s="13" t="s">
         <v>14</v>
@@ -5550,19 +5550,19 @@
         <v>8</v>
       </c>
       <c r="G85" s="20" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H85" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I85" s="14" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="J85" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K85" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>